<commit_message>
update upload api doc
</commit_message>
<xml_diff>
--- a/server/documents/api/Upload.xlsx
+++ b/server/documents/api/Upload.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21615"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="492" documentId="11_92480E3D80EBD8D2623DC6FA873E8C18510380D4" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{FC037ACE-70D6-4078-B15D-8054C2DF1C9E}"/>
+  <xr:revisionPtr revIDLastSave="494" documentId="11_92480E3D80EBD8D2623DC6FA873E8C18510380D4" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{ADDBEE16-C5D1-4019-AA28-255E5CF96ACC}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -152,7 +152,7 @@
     <t>Upload multiple image</t>
   </si>
   <si>
-    <t>/api/upload_images</t>
+    <t>/upload/upload_images</t>
   </si>
   <si>
     <t>image1</t>
@@ -176,7 +176,7 @@
     <t>http://localhost:3000/upload/upload_images</t>
   </si>
   <si>
-    <t>["ok", "ok", "ok", "ok", "ok"]</t>
+    <t>["ok", "ok", "ok", "ok", "ok", "ok"]</t>
   </si>
   <si>
     <t>["ok", "ok", "fail", "fail", "ok"]</t>
@@ -601,75 +601,75 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -989,7 +989,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1031,52 +1031,52 @@
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="50"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="60"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="50"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="60"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="52"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="62"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="55"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="65"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="56" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1096,7 +1096,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
-      <c r="A9" s="66"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="16" t="s">
         <v>19</v>
       </c>
@@ -1110,7 +1110,7 @@
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="14.25">
-      <c r="A10" s="66"/>
+      <c r="A10" s="57"/>
       <c r="B10" s="4" t="s">
         <v>22</v>
       </c>
@@ -1124,7 +1124,7 @@
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1">
-      <c r="A11" s="63"/>
+      <c r="A11" s="58"/>
       <c r="B11" s="12"/>
       <c r="C11" s="3"/>
       <c r="D11" s="25"/>
@@ -1132,7 +1132,7 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="40.5" customHeight="1">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="47" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="44" t="s">
@@ -1141,14 +1141,14 @@
       <c r="C12" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="67" t="s">
+      <c r="D12" s="50" t="s">
         <v>27</v>
       </c>
       <c r="E12" s="26"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="46" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="13" t="s">
@@ -1160,7 +1160,7 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="14.25">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="11"/>
@@ -1170,7 +1170,7 @@
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="42.75" customHeight="1">
-      <c r="A15" s="57"/>
+      <c r="A15" s="54"/>
       <c r="B15" s="20"/>
       <c r="C15" s="39" t="s">
         <v>31</v>
@@ -1182,7 +1182,7 @@
       <c r="F15" s="42"/>
     </row>
     <row r="16" spans="1:6" ht="42.75" customHeight="1">
-      <c r="A16" s="57"/>
+      <c r="A16" s="54"/>
       <c r="B16" s="21"/>
       <c r="C16" s="43" t="s">
         <v>33</v>
@@ -1194,7 +1194,7 @@
       <c r="F16" s="17"/>
     </row>
     <row r="17" spans="1:6" ht="42.75" customHeight="1">
-      <c r="A17" s="57"/>
+      <c r="A17" s="54"/>
       <c r="B17" s="21"/>
       <c r="C17" s="32" t="s">
         <v>35</v>
@@ -1206,7 +1206,7 @@
       <c r="F17" s="19"/>
     </row>
     <row r="18" spans="1:6" ht="42.75" customHeight="1">
-      <c r="A18" s="57"/>
+      <c r="A18" s="54"/>
       <c r="B18" s="17"/>
       <c r="C18" s="43" t="s">
         <v>37</v>
@@ -1218,7 +1218,7 @@
       <c r="F18" s="34"/>
     </row>
     <row r="19" spans="1:6" ht="42.75" customHeight="1">
-      <c r="A19" s="58"/>
+      <c r="A19" s="55"/>
       <c r="B19" s="14"/>
       <c r="C19" s="35" t="s">
         <v>39</v>
@@ -1251,7 +1251,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AB08B871-319A-5E8F-9EB7-4F8AD09F5AD4}">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1293,52 +1293,52 @@
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="50"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="60"/>
     </row>
     <row r="5" spans="1:6" ht="15">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="50"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="60"/>
     </row>
     <row r="6" spans="1:6" ht="15">
       <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="52"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="62"/>
     </row>
     <row r="7" spans="1:6" ht="15">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="55"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="65"/>
     </row>
     <row r="8" spans="1:6" ht="15">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="66" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1358,7 +1358,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
-      <c r="A9" s="47"/>
+      <c r="A9" s="67"/>
       <c r="B9" s="16" t="s">
         <v>43</v>
       </c>
@@ -1372,7 +1372,7 @@
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1">
-      <c r="A10" s="59"/>
+      <c r="A10" s="68"/>
       <c r="B10" s="23" t="s">
         <v>45</v>
       </c>
@@ -1386,7 +1386,7 @@
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1">
-      <c r="A11" s="59"/>
+      <c r="A11" s="68"/>
       <c r="B11" s="27" t="s">
         <v>46</v>
       </c>
@@ -1400,7 +1400,7 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1">
-      <c r="A12" s="48"/>
+      <c r="A12" s="69"/>
       <c r="B12" s="25" t="s">
         <v>47</v>
       </c>
@@ -1414,7 +1414,7 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="48"/>
+      <c r="A13" s="69"/>
       <c r="B13" s="4" t="s">
         <v>48</v>
       </c>
@@ -1428,31 +1428,31 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="15">
-      <c r="A14" s="60"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="12"/>
       <c r="C14" s="28"/>
-      <c r="D14" s="69"/>
+      <c r="D14" s="52"/>
       <c r="E14" s="27"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="40.5" customHeight="1">
-      <c r="A15" s="65" t="s">
+      <c r="A15" s="48" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="68" t="s">
+      <c r="C15" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="67" t="s">
+      <c r="D15" s="50" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="16"/>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" ht="15">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="46" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="13" t="s">
@@ -1464,7 +1464,7 @@
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="11"/>
@@ -1474,7 +1474,7 @@
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="42.75" customHeight="1">
-      <c r="A18" s="57"/>
+      <c r="A18" s="54"/>
       <c r="B18" s="20"/>
       <c r="C18" s="39" t="s">
         <v>31</v>
@@ -1486,7 +1486,7 @@
       <c r="F18" s="42"/>
     </row>
     <row r="19" spans="1:6" ht="42.75" customHeight="1">
-      <c r="A19" s="57"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="21"/>
       <c r="C19" s="43" t="s">
         <v>31</v>
@@ -1498,7 +1498,7 @@
       <c r="F19" s="17"/>
     </row>
     <row r="20" spans="1:6" ht="42.75" customHeight="1">
-      <c r="A20" s="57"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="21"/>
       <c r="C20" s="32" t="s">
         <v>35</v>
@@ -1510,7 +1510,7 @@
       <c r="F20" s="19"/>
     </row>
     <row r="21" spans="1:6" ht="42.75" customHeight="1">
-      <c r="A21" s="57"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="17"/>
       <c r="C21" s="43" t="s">
         <v>37</v>
@@ -1522,7 +1522,7 @@
       <c r="F21" s="34"/>
     </row>
     <row r="22" spans="1:6" ht="42.75" customHeight="1">
-      <c r="A22" s="58"/>
+      <c r="A22" s="55"/>
       <c r="B22" s="14"/>
       <c r="C22" s="35" t="s">
         <v>33</v>

</xml_diff>